<commit_message>
[ELEC] BOM - gen BOM and added parameters to parts
</commit_message>
<xml_diff>
--- a/Electrical/MLB_REV1/Project Outputs for MLB_REV1/MLB_REV1.xlsx
+++ b/Electrical/MLB_REV1/Project Outputs for MLB_REV1/MLB_REV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\mattrics\Electrical\MLB_REV1\Project Outputs for MLB_REV1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01EFA92C-A3B6-436D-8068-EA6487044DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00981FE9-9984-426B-BBF8-6DCECE661E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{042A4470-142A-4E0A-8CD5-879B058159B6}"/>
+    <workbookView xWindow="5760" yWindow="24" windowWidth="17280" windowHeight="8964" xr2:uid="{0EA69168-D3D9-40D4-917A-BBD3E708F007}"/>
   </bookViews>
   <sheets>
     <sheet name="MLB_REV1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="239">
   <si>
     <t>Line #</t>
   </si>
@@ -75,7 +75,7 @@
     <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0805, 10uF, X7R, 15%, 10%, 10V</t>
   </si>
   <si>
-    <t>C1, C5, C22</t>
+    <t>C1, C5, C22, C49</t>
   </si>
   <si>
     <t>Murata Electronics</t>
@@ -105,7 +105,7 @@
     <t>CL21 Series 0805 1uF 16V ±10% Tolerance X7R Multilayer Ceramic Chip Capacitor</t>
   </si>
   <si>
-    <t>C3, C12, C13</t>
+    <t>C3, C24, C26, C42, C45, C48, C51</t>
   </si>
   <si>
     <t>Samsung Electro-Mechanics</t>
@@ -114,28 +114,55 @@
     <t>1276-1026-1-ND</t>
   </si>
   <si>
-    <t>GQM2195C2E140JB12D</t>
-  </si>
-  <si>
-    <t>Ceramic Capacitor 14pF ±5% 250VDC C0G 0805 Paper T/R</t>
-  </si>
-  <si>
-    <t>C6, C7</t>
-  </si>
-  <si>
-    <t>490-GQM2195C2E140JB12DCT-ND</t>
-  </si>
-  <si>
-    <t>CL21B104KBCNNNC</t>
-  </si>
-  <si>
-    <t>CL21 Series 0805 100nF 50V ±10% Tolerance X7R Multilayer Ceramic Chip Capacitor</t>
-  </si>
-  <si>
-    <t>C8, C9, C10, C11, C14</t>
-  </si>
-  <si>
-    <t>1276-1003-1-ND</t>
+    <t>GJM1555C1H140GB01D</t>
+  </si>
+  <si>
+    <t>Multi-Layer Ceramic Capacitor 14pF C0G  ±2% 0402 Paper T/R</t>
+  </si>
+  <si>
+    <t>C6, C9</t>
+  </si>
+  <si>
+    <t>490-14443-1-ND</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R7BB104</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>C7, C10, C11, C12, C13, C16, C39</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>311-1338-1-ND</t>
+  </si>
+  <si>
+    <t>GRM155R60J106ME05D</t>
+  </si>
+  <si>
+    <t>Chip Multilayer Ceramic Capacitors for General Purpose, 0402, 10uF, X5R, 15%, 20%, 6.3V</t>
+  </si>
+  <si>
+    <t>C8, C14</t>
+  </si>
+  <si>
+    <t>490-GRM155R60J106ME05DCT-ND</t>
+  </si>
+  <si>
+    <t>CC0402KRX5R5BB105</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 6.3V X5R 0402</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>311-1438-1-ND</t>
   </si>
   <si>
     <t>C0805C104M3RACTU</t>
@@ -144,7 +171,7 @@
     <t>CAP CER 0.1UF 25V 20% X7R 0805</t>
   </si>
   <si>
-    <t>C15, C16, C17, C18, C19, C20, C21, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45</t>
+    <t>C17, C18, C19, C20, C21, C23, C25, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38, C40, C41, C43, C44, C46, C47, C50</t>
   </si>
   <si>
     <t>KEMET</t>
@@ -153,102 +180,90 @@
     <t>399-C0805C104M3RAC7800CT-ND</t>
   </si>
   <si>
-    <t>UWR1A101MCL1GB</t>
+    <t>DF2S10FS,L3M</t>
+  </si>
+  <si>
+    <t>TVS DIODE 8VWM FSC</t>
+  </si>
+  <si>
+    <t>D1, D17, D18, D19</t>
+  </si>
+  <si>
+    <t>Toshiba Semiconductor and Storage</t>
+  </si>
+  <si>
+    <t>DF2S10FSL3MCT-ND</t>
+  </si>
+  <si>
+    <t>MM3Z8V2ST1G</t>
+  </si>
+  <si>
+    <t>Zener Voltage Regulator, 300 mW, Tight Tolerance Portfolio, 2-Pin SOD-323, Pb-Free, Tape and Reel</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>On Semiconductor</t>
+  </si>
+  <si>
+    <t>MM3Z8V2ST1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>SP7538PUTG</t>
+  </si>
+  <si>
+    <t>ESD Suppressor TVS Octal Uni-Dir 25kV 9-Pin UDFN T/R</t>
+  </si>
+  <si>
+    <t>D3, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16</t>
+  </si>
+  <si>
+    <t>Littelfuse</t>
+  </si>
+  <si>
+    <t>F7417CT-ND</t>
+  </si>
+  <si>
+    <t>EAST1616RGBB4</t>
+  </si>
+  <si>
+    <t>LED RGB CLEAR 4SMD</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Everlight Electronics Co Ltd</t>
+  </si>
+  <si>
+    <t>1080-1552-1-ND</t>
+  </si>
+  <si>
+    <t>598-8170-107F</t>
+  </si>
+  <si>
+    <t>Single Color, 2 V, -30 to 85 degC, 2-Pin SMD (0805), RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>DS1</t>
+  </si>
+  <si>
+    <t>Dialight</t>
+  </si>
+  <si>
+    <t>5988170107F</t>
+  </si>
+  <si>
+    <t>350-2044-1-ND</t>
+  </si>
+  <si>
+    <t>MFS101D-8-Z</t>
   </si>
   <si>
     <t>No Description Available</t>
   </si>
   <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>Nichicon</t>
-  </si>
-  <si>
-    <t>493-14561-1-ND</t>
-  </si>
-  <si>
-    <t>DF2S10FS,L3M</t>
-  </si>
-  <si>
-    <t>TVS DIODE 8VWM FSC</t>
-  </si>
-  <si>
-    <t>D1, D17, D18, D19</t>
-  </si>
-  <si>
-    <t>Toshiba Semiconductor and Storage</t>
-  </si>
-  <si>
-    <t>DF2S10FSL3MCT-ND</t>
-  </si>
-  <si>
-    <t>MM3Z8V2ST1G</t>
-  </si>
-  <si>
-    <t>Zener Voltage Regulator, 300 mW, Tight Tolerance Portfolio, 2-Pin SOD-323, Pb-Free, Tape and Reel</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>On Semiconductor</t>
-  </si>
-  <si>
-    <t>MM3Z8V2ST1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>SP7538PUTG</t>
-  </si>
-  <si>
-    <t>ESD Suppressor TVS Octal Uni-Dir 25kV 9-Pin UDFN T/R</t>
-  </si>
-  <si>
-    <t>D3, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16</t>
-  </si>
-  <si>
-    <t>Littelfuse</t>
-  </si>
-  <si>
-    <t>F7417CT-ND</t>
-  </si>
-  <si>
-    <t>EAST1616RGBB4</t>
-  </si>
-  <si>
-    <t>LED RGB CLEAR 4SMD</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>Everlight Electronics Co Ltd</t>
-  </si>
-  <si>
-    <t>1080-1552-1-ND</t>
-  </si>
-  <si>
-    <t>598-8170-107F</t>
-  </si>
-  <si>
-    <t>Single Color, 2 V, -30 to 85 degC, 2-Pin SMD (0805), RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>DS1</t>
-  </si>
-  <si>
-    <t>Dialight</t>
-  </si>
-  <si>
-    <t>5988170107F</t>
-  </si>
-  <si>
-    <t>350-2044-1-ND</t>
-  </si>
-  <si>
-    <t>MFS101D-8-Z</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -279,7 +294,7 @@
     <t>Connector Header Through Hole 2 position</t>
   </si>
   <si>
-    <t>J3, J6, J7, J8, J11, J13, J15, J17, J19, J23, J25, J27</t>
+    <t>J3, J8, J9, J10, J11, J12, J13, J15, J18, J19, J22, J25, J28, J29</t>
   </si>
   <si>
     <t>TE Connectivity AMP Connectors</t>
@@ -309,7 +324,7 @@
     <t>CONN JUMPER SHORTING .100" GOLD</t>
   </si>
   <si>
-    <t>J5, J12, J14, J16, J18, J20, J22, J26, J28</t>
+    <t>J5, J7, J14, J16, J17, J20, J21, J26, J27, J30</t>
   </si>
   <si>
     <t>Sullins</t>
@@ -324,7 +339,7 @@
     <t>CONN HDR 8POS 0.1 TIN PCB</t>
   </si>
   <si>
-    <t>J9, J10</t>
+    <t>J6</t>
   </si>
   <si>
     <t>Sullins Connector Solutions</t>
@@ -336,7 +351,7 @@
     <t>1-787082-8</t>
   </si>
   <si>
-    <t>J21</t>
+    <t>J23</t>
   </si>
   <si>
     <t>A35091-ND</t>
@@ -384,13 +399,25 @@
     <t>785-1016-1-ND</t>
   </si>
   <si>
+    <t>RK7002BMT116</t>
+  </si>
+  <si>
+    <t>Q2, Q3, Q4</t>
+  </si>
+  <si>
+    <t>Rohm Semiconductor</t>
+  </si>
+  <si>
+    <t>RK7002BMT116CT-ND</t>
+  </si>
+  <si>
     <t>RC0805FR-0710KL</t>
   </si>
   <si>
     <t>Chip Resistor, 10 KOhm, +/- 1%, 0.125 W, -55 to 155 degC, 0805 (2012 Metric), RoHS, Tape and Reel</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R13, R14, R15, R21, R23, R26, R27, R28, R29, R30, R31, R57, R103, R108, R109</t>
+    <t>R1, R2, R3, R4, R13, R14, R15, R22, R25, R28, R29, R30, R31, R32, R34, R53, R76, R81, R82</t>
   </si>
   <si>
     <t>Yageo</t>
@@ -402,7 +429,7 @@
     <t>100Ω ±1% 0.125W 0805 Thick Film Chip Resistor AEC-Q200 compliant</t>
   </si>
   <si>
-    <t>R5, R12, R35, R36, R41, R44, R47</t>
+    <t>R5, R12, R37, R38, R40, R41, R43, R44, R47, R48, R54</t>
   </si>
   <si>
     <t>Stackpole Electronics Inc</t>
@@ -429,7 +456,7 @@
     <t>RES 0 OHM JUMPER 1/8W 0805</t>
   </si>
   <si>
-    <t>R10, R17, R20, R25, R33, R34, R38, R39, R102, R105, R112, R114, R116, R117, R118, R119, R120, R121</t>
+    <t>R10, R17, R20, R27, R33, R35, R74, R75, R85, R88, R89, R91, R92, R94</t>
   </si>
   <si>
     <t>RMCF0805ZT0R00CT-ND</t>
@@ -441,7 +468,7 @@
     <t>Chip Resistor, 1 KOhm, +/- 1%, 125 mW, -55 to 155 degC, 0805 (2012 Metric), RoHS, Tape and Reel</t>
   </si>
   <si>
-    <t>R11, R104, R106</t>
+    <t>R11, R18, R19, R77, R79</t>
   </si>
   <si>
     <t>311-1.00KCRCT-ND</t>
@@ -450,7 +477,7 @@
     <t>ERJ-6ENF5100V</t>
   </si>
   <si>
-    <t>R16, R22</t>
+    <t>R16, R24</t>
   </si>
   <si>
     <t>Panasonic</t>
@@ -459,31 +486,34 @@
     <t>P510CCT-ND</t>
   </si>
   <si>
-    <t>ERJ6ENF2200V</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>P220CCT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0805FG1M00</t>
-  </si>
-  <si>
-    <t>1MΩ ±1% 0.125W 0805 Thick Film Chip Resistor AEC-Q200 compliant</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>RMCF0805FG1M00CT-ND</t>
+    <t>CRGCQ0402F1M0</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0402 1M Ohm 1% 0.063W(1/16W) ±100ppm/C Pad SMD Automotive T/R</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>TE Connectivity Passive Product</t>
+  </si>
+  <si>
+    <t>A129663CT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-07220RL</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>311-220LRCT-ND</t>
   </si>
   <si>
     <t>CRCW080515K0FKTA</t>
   </si>
   <si>
-    <t>R24, R32, R42, R45, R48, R49, R50, R51, R52, R53, R54, R55, R56, R59, R61, R62, R63, R64, R65, R66, R67, R68, R69, R70, R71, R72, R73, R74, R75, R76, R77, R78, R79, R80, R81, R82, R83, R84, R85, R86, R87, R88, R89, R90, R91, R92, R93, R94, R95, R96, R97, R98, R99, R100, R101</t>
+    <t>R26, R36, R42, R45, R46, R49, R51, R52, R56, R57, R58, R59, R60, R61, R62, R63, R64, R65, R66, R67, R68, R69, R70, R71, R72, R73</t>
   </si>
   <si>
     <t>Vishay Dale</t>
@@ -498,34 +528,19 @@
     <t>Chip Resistor, 300 Ohm, +/- 1%, 0.125 W, -55 to 155 degC, 0805 (2012 Metric), RoHS, Tape and Reel</t>
   </si>
   <si>
-    <t>R37</t>
+    <t>R39</t>
   </si>
   <si>
     <t>P300CCT-ND</t>
   </si>
   <si>
-    <t>RK7002BMT116</t>
-  </si>
-  <si>
-    <t>R40, R43, R46</t>
-  </si>
-  <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
-    <t>RK7002BMT116CT-ND</t>
-  </si>
-  <si>
     <t>CRGCQ0805F68K</t>
   </si>
   <si>
     <t>CRGCQ0805 68KΩ 0.125W ±100ppm/°C 1% 150V</t>
   </si>
   <si>
-    <t>R58</t>
-  </si>
-  <si>
-    <t>TE Connectivity Passive Product</t>
+    <t>R50</t>
   </si>
   <si>
     <t>A129771CT-ND</t>
@@ -537,10 +552,7 @@
     <t>20K 0.125W 1% 0805 (2012 Metric)  SMD</t>
   </si>
   <si>
-    <t>R60, R110</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
+    <t>R55, R83</t>
   </si>
   <si>
     <t>RC0805FR-0720KL</t>
@@ -552,7 +564,7 @@
     <t>ERJ-6GEYJ333V</t>
   </si>
   <si>
-    <t>R107, R111</t>
+    <t>R80, R84</t>
   </si>
   <si>
     <t>P33KACT-ND</t>
@@ -564,7 +576,7 @@
     <t>RES Thick Film, 5.1kΩ, 1%, 0.125W, 100ppm/°C, 0805</t>
   </si>
   <si>
-    <t>R113</t>
+    <t>R86</t>
   </si>
   <si>
     <t>CRCW08055K10FKEAC</t>
@@ -579,13 +591,13 @@
     <t>Chip Resistor, 470 Ohm, +/- 1%, 125 mW, -55 to 155 degC, 0805 (2012 Metric), RoHS, Tape and Reel</t>
   </si>
   <si>
-    <t>R115</t>
+    <t>R87</t>
   </si>
   <si>
     <t>311-470CRCT-ND</t>
   </si>
   <si>
-    <t>503398-1892</t>
+    <t>5033981892</t>
   </si>
   <si>
     <t>Micro SD Connector, Pitch 1.1 mm, 8 Position, Height 1.4 mm, -25 to 85 degC, RoHS, Tape and Reel</t>
@@ -594,9 +606,6 @@
     <t>SD1</t>
   </si>
   <si>
-    <t>5033981892</t>
-  </si>
-  <si>
     <t>WM11190CT-ND</t>
   </si>
   <si>
@@ -624,7 +633,7 @@
     <t>Natural PC Test Point , Plating Surface Mount Mounting Type</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, TP33, TP34, TP35, TP36, TP37, TP38, TP39, TP40, TP41, TP42, TP43, TP44, TP45, TP46, TP47, TP48, TP49, TP50, TP51, TP52, TP53, TP54, TP55, TP56, TP57, TP58, TP59, TP60, TP61, TP62, TP63, TP64, TP65, TP66, TP67, TP68, TP69, TP70, TP71, TP72, TP73, TP74, TP75, TP76, TP77, TP78, TP79, TP80, TP81, TP82, TP83, TP84, TP85, TP86, TP87, TP88, TP89, TP90, TP91, TP92, TP93, TP94, TP95, TP96, TP97, TP98, TP99, TP100, TP101, TP102, TP103, TP104, TP105, TP106, TP107, TP108, TP109, TP110, TP111, TP112, TP113, TP114, TP115, TP116, TP117, TP118, TP119, TP120, TP121, TP122, TP123, TP124, TP125, TP126, TP127, TP128, TP129, TP130, TP131, TP132, TP133, TP134, TP135, TP136, TP137, TP138, TP139, TP140, TP141, TP142, TP143, TP144, TP145, TP146, TP147, TP148, TP149, TP150, TP151, TP152, TP153, TP154, TP155, TP156, TP157, TP158, TP159, TP160, TP161, TP162, TP163, TP164, TP165, TP166, TP167, TP168, TP169, TP170, TP171, TP172, TP173, TP174, TP175, TP176, TP177, TP178, TP179, TP180, TP181, TP182, TP183, TP184, TP185, TP186, TP187, TP188, TP189, TP190, TP191, TP192, TP193, TP194</t>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, TP33, TP34, TP35, TP36, TP37, TP38, TP39, TP40, TP41, TP42, TP43, TP44, TP45, TP46, TP47, TP48, TP49, TP50, TP51, TP52, TP53, TP54, TP55, TP56, TP57, TP58, TP59, TP60, TP61, TP62, TP63, TP64, TP65, TP66, TP67, TP68, TP69, TP70, TP71, TP72, TP73, TP74, TP75, TP76, TP77, TP78, TP79, TP80, TP81, TP82, TP83, TP84, TP85</t>
   </si>
   <si>
     <t>A106145CT-ND</t>
@@ -663,13 +672,43 @@
     <t>511-STM32L152RBT6A</t>
   </si>
   <si>
+    <t>AP22615AWU-7</t>
+  </si>
+  <si>
+    <t>Integrated Circuit</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>AP22615AWU-7DICT-ND</t>
+  </si>
+  <si>
+    <t>MCP6411T-E/OT</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 1 CIRCUIT SOT23-5</t>
+  </si>
+  <si>
+    <t>U4, U18, U19, U20</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>MCP6411T-E/OTCT-ND</t>
+  </si>
+  <si>
     <t>NX3L4051PW,118</t>
   </si>
   <si>
     <t>1 Circuit IC Switch 8:1 750mOhm 16-TSSOP</t>
   </si>
   <si>
-    <t>U3, U4, U7, U8, U9, U10, U11, U12, U13, U14, U15, U16</t>
+    <t>U5, U6, U7, U8, U9, U10, U11, U12, U13, U14, U15, U16</t>
   </si>
   <si>
     <t>NXP USA Inc.</t>
@@ -678,36 +717,6 @@
     <t>568-12393-1-ND</t>
   </si>
   <si>
-    <t>AP22615AWU-7</t>
-  </si>
-  <si>
-    <t>Integrated Circuit</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>Diodes Inc.</t>
-  </si>
-  <si>
-    <t>AP22615AWU-7DICT-ND</t>
-  </si>
-  <si>
-    <t>MCP6401RT-E/OT</t>
-  </si>
-  <si>
-    <t>IC, OP-AMP, 1MHZ, 0.5V/Âµs</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>MCP6476RT-E/OT</t>
-  </si>
-  <si>
-    <t>150-MCP6476RT-E/OTCT-ND</t>
-  </si>
-  <si>
     <t>MCP6N11T-001E/MNY</t>
   </si>
   <si>
@@ -720,31 +729,19 @@
     <t>MCP6N11T-001E/MNYCT-ND</t>
   </si>
   <si>
-    <t>TLV272QDRQ1</t>
-  </si>
-  <si>
-    <t>Automotive Catalog 550 uA/Ch, 3 MHz, Rail-to-Rail Output Operational Amplifier, 2.7 to 16 V, -40 to 125 degC, 8-pin SOIC (D8), Green (RoHS &amp; no Sb/Br)</t>
-  </si>
-  <si>
-    <t>U18, U19</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>Digi-key</t>
-  </si>
-  <si>
-    <t>296-17870-1-ND</t>
-  </si>
-  <si>
-    <t>ADS1110A2IDBVR</t>
-  </si>
-  <si>
-    <t>16-Bit Delta-Sigma ADC with Internal Reference, PGA and Oscillator, I2C Serial Interface, -40 to 85 degC, 6-pin SOT23 (DBV6), Green (RoHS &amp; no Sb/Br)</t>
-  </si>
-  <si>
-    <t>U20</t>
+    <t>MCP3221A7T-E/OT</t>
+  </si>
+  <si>
+    <t>Low Power 12-Bit A/D Converter With I2C Interface, 5-Pin SOT-23, Extended Temperature, Tape and Reel</t>
+  </si>
+  <si>
+    <t>U21</t>
+  </si>
+  <si>
+    <t>MCP3221A7T-E/OTCT-ND</t>
+  </si>
+  <si>
+    <t>ECS-200-9-33B-CKY-TR</t>
   </si>
   <si>
     <t>Crystal 20MHz Â±10ppm (Tol) Â±10ppm (Stability) 9pF FUND 40Ohm 4-Pin Mini-CSMD T/R</t>
@@ -754,9 +751,6 @@
   </si>
   <si>
     <t>ECS Inc.</t>
-  </si>
-  <si>
-    <t>ECS-200-9-33B-CKY-TR</t>
   </si>
   <si>
     <t>XC2464CT-ND</t>
@@ -1141,7 +1135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C03E41-9810-4545-BAFE-9AEDA795B9E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4D3EBC-B3E0-4923-B749-3181E08A0CE1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1205,7 +1199,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -1263,7 +1257,7 @@
         <v>22</v>
       </c>
       <c r="E4" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>23</v>
@@ -1307,7 +1301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1321,10 +1315,10 @@
         <v>31</v>
       </c>
       <c r="E6" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>29</v>
@@ -1333,30 +1327,30 @@
         <v>14</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>14</v>
@@ -1366,9 +1360,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1382,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>38</v>
@@ -1391,94 +1383,94 @@
         <v>14</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="4">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="4">
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="4">
-        <v>13</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1486,80 +1478,78 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="4">
+        <v>13</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E14" s="4">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>14</v>
@@ -1568,7 +1558,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1597,10 +1587,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
         <v>78</v>
       </c>
@@ -1611,7 +1599,7 @@
         <v>80</v>
       </c>
       <c r="E16" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>81</v>
@@ -1626,7 +1614,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -1640,7 +1628,7 @@
         <v>85</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>86</v>
@@ -1669,7 +1657,7 @@
         <v>90</v>
       </c>
       <c r="E18" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>91</v>
@@ -1684,7 +1672,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
@@ -1698,7 +1686,7 @@
         <v>95</v>
       </c>
       <c r="E19" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>96</v>
@@ -1714,23 +1702,21 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>98</v>
@@ -1739,47 +1725,47 @@
         <v>14</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="H21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>107</v>
@@ -1788,10 +1774,10 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>14</v>
@@ -1800,7 +1786,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1817,10 +1803,10 @@
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>14</v>
@@ -1829,7 +1815,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -1843,7 +1829,7 @@
         <v>117</v>
       </c>
       <c r="E24" s="4">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>118</v>
@@ -1855,30 +1841,30 @@
         <v>14</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>120</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E25" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>122</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>14</v>
@@ -1901,10 +1887,10 @@
         <v>126</v>
       </c>
       <c r="E26" s="4">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>124</v>
@@ -1913,7 +1899,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1930,10 +1916,10 @@
         <v>130</v>
       </c>
       <c r="E27" s="4">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>128</v>
@@ -1942,7 +1928,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -1950,269 +1936,267 @@
         <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" s="4">
-        <v>3</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="H28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>9</v>
+        <v>138</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" s="4">
+        <v>14</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E29" s="4">
+      <c r="H29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="4">
+        <v>5</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="4">
         <v>2</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E30" s="4">
+      <c r="F31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="4">
         <v>1</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" s="4">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" s="4">
-        <v>55</v>
-      </c>
       <c r="F32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="H32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
       <c r="B33" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>138</v>
+        <v>32</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E34" s="4">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="H34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E35" s="4">
         <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="4">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E36" s="4">
-        <v>2</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="3" t="s">
+    </row>
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>171</v>
@@ -2221,68 +2205,68 @@
         <v>2</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>138</v>
+        <v>32</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>175</v>
       </c>
       <c r="E38" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G38" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="3" t="s">
+    </row>
+    <row r="39" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>14</v>
@@ -2308,159 +2292,159 @@
         <v>1</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="3" t="s">
+    </row>
+    <row r="41" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="4">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E41" s="4">
+    </row>
+    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" s="4">
         <v>2</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="H42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E42" s="4">
-        <v>194</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="3" t="s">
+    </row>
+    <row r="43" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="4">
+        <v>85</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E43" s="4">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="H44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="3" t="s">
+      <c r="E45" s="4">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="G45" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H45" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="I45" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="E45" s="4">
-        <v>12</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2468,28 +2452,28 @@
         <v>9</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="E46" s="4">
         <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2497,28 +2481,28 @@
         <v>9</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="E47" s="4">
+        <v>4</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="G47" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="E47" s="4">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2526,118 +2510,116 @@
         <v>9</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="E48" s="4">
+        <v>12</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="G48" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="E48" s="4">
+    </row>
+    <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E49" s="4">
         <v>1</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I48" s="3" t="s">
+      <c r="F49" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="H49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E49" s="4">
-        <v>2</v>
-      </c>
-      <c r="F49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="E50" s="4">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I50" s="4"/>
     </row>
     <row r="51" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A51" s="4"/>
       <c r="B51" s="3" t="s">
-        <v>9</v>
+        <v>234</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="E51" s="4">
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="19" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup scale="22" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>